<commit_message>
Updated map and gt.
</commit_message>
<xml_diff>
--- a/Data/Voter_Registration_By_County_and_Party_Feb_2019.xlsx
+++ b/Data/Voter_Registration_By_County_and_Party_Feb_2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debis\Documents\R_Projects\Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debis\Documents\R_Projects\Final_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{319F029E-34FF-42D9-8426-F6DB131F330D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56335A6B-4648-4DFF-9DCD-E2F440D95395}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20ECE57A-2022-4F93-8A7D-405D627E2D18}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>  Columbia  </t>
   </si>
   <si>
-    <t>  Desoto  </t>
-  </si>
-  <si>
     <t>  Dixie  </t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Data as of February 28, 2019.</t>
+  </si>
+  <si>
+    <t>  DeSoto  </t>
   </si>
 </sst>
 </file>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A28DED5-3915-4A05-ADF1-3304F8DF2CFB}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>5842</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>4114</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>220816</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="17" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>96003</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>34673</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>2786</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>4771</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>6729</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>2901</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>5089</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>2573</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>5496</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>6579</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>56128</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>27996</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>271789</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>6362</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>52932</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>10685</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>3293</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>1909</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>105357</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>194401</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>57336</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>13247</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>1015</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>3730</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>107228</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>109312</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>56760</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>377967</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>20961</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>39127</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <v>79594</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>9251</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>214110</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>48749</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>266481</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52">
         <v>137234</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53">
         <v>235913</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54">
         <v>152348</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>19685</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>79297</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>135880</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>111494</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59">
         <v>99073</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>65889</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>53553</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>12435</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>4898</v>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64">
         <v>3502</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>135211</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>9089</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>30732</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="68" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68">
         <v>8435</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>4718813</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>